<commit_message>
Removed day of match
</commit_message>
<xml_diff>
--- a/eventData/users.xlsx
+++ b/eventData/users.xlsx
@@ -646,7 +646,11 @@
           <t>d3b9b1ead0952a666172506122c39bfa2086869215486c56217a9f64a86b538d</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['Scotland', 1, 2]</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>

</xml_diff>

<commit_message>
Added users and fixtures data
</commit_message>
<xml_diff>
--- a/eventData/users.xlsx
+++ b/eventData/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,7 +648,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['Scotland', 1, 2]</t>
+          <t>['Germany', 4, 0]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -961,19 +961,71 @@
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['Spain', 3, 1]</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['Italy', 4, 1]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['Netherlands', 0, 2]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>['Draw', 1, 1]</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['England', 1, 3]</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>['Ukraine', 1, 2]</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>['Belgium', 1, 0]</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['France', 1, 3]</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>['Turkey', 3, 1]</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>['Portugal', 4, 1]</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>['Croatia', 3, 0]</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>['Germany', 3, 1]</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>['Switzerland', 1, 3]</t>
+        </is>
+      </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
@@ -1287,6 +1339,246 @@
       <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MonaliPa</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>monalipatel2123@gmail.com</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4a4c777a3b0b098a170aa72d97892ab1632944814a6a393ddbcb0cdc74f84b30</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['Germany', 3, 0]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PlayerOne gg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>rvce.karan@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>17f80754644d33ac685b0842a402229adbb43fc9312f7bdf36ba24237a1f1ffb</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['Germany', 2, 1]</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['Draw', 1, 1]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['Spain', 2, 1]</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['Italy', 2, 1]</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['Netherlands', 1, 2]</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>['Denmark', 0, 2]</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>['England', 0, 3]</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>meghapriya22@gmail.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>meghapriya22@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>f4786924bb3a391712c02d47dc9678783fb14604f066e55fa5f0277d89c74496</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['Germany', 3, 0]</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the users list and modified leaderboard display
</commit_message>
<xml_diff>
--- a/eventData/users.xlsx
+++ b/eventData/users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\eventData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\exportData\ineos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF31AD9-4E1F-48F7-9080-8B9511D095E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1760AB70-8B0D-4CEA-AA1C-6EDA99FDCB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="274">
   <si>
     <t>username</t>
   </si>
@@ -160,6 +160,9 @@
     <t>['Turkey', 2, 0]</t>
   </si>
   <si>
+    <t>['Czech Republic', 1, 2]</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -547,9 +550,6 @@
     <t>['Scotland', 2, 0]</t>
   </si>
   <si>
-    <t>Geoff</t>
-  </si>
-  <si>
     <t>geoff.gough9a@gmail.com</t>
   </si>
   <si>
@@ -832,7 +832,16 @@
     <t>68a132f43a4c8241d5049b975d694743357d0c4df8ce249e9936009b847ccb1a</t>
   </si>
   <si>
-    <t>['Czech Republic', 1, 2]</t>
+    <t>GeoffG</t>
+  </si>
+  <si>
+    <t>b11dedb1e7de81f80eb743dc6326aab69a902f66379424db74a06032ea7054ed</t>
+  </si>
+  <si>
+    <t>['France', 0, 1]</t>
+  </si>
+  <si>
+    <t>['Georgia', 2, 0]</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1207,7 @@
   <dimension ref="A1:AM32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,21 +1394,24 @@
       <c r="N2" t="s">
         <v>45</v>
       </c>
+      <c r="Y2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -1407,266 +1419,266 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" t="s">
+        <v>70</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA5" t="s">
         <v>61</v>
       </c>
-      <c r="N5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>68</v>
-      </c>
-      <c r="U5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="AB5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>69</v>
       </c>
-      <c r="W5" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>68</v>
-      </c>
       <c r="AK5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AL5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N6" t="s">
         <v>45</v>
       </c>
       <c r="O6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AA6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AC6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL6" t="s">
         <v>98</v>
       </c>
-      <c r="AE6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>97</v>
-      </c>
       <c r="AM6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M7" t="s">
         <v>44</v>
@@ -1675,1638 +1687,1659 @@
         <v>45</v>
       </c>
       <c r="O7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="T7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="V7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="W7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Y7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AA7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AB7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AD7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AE7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AF7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AH7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AI7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AK7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AL7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AM7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" t="s">
+        <v>130</v>
+      </c>
+      <c r="O8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" t="s">
         <v>94</v>
       </c>
-      <c r="E8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="Q8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L8" t="s">
-        <v>90</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="R8" t="s">
+        <v>131</v>
+      </c>
+      <c r="T8" t="s">
+        <v>132</v>
+      </c>
+      <c r="U8" t="s">
+        <v>133</v>
+      </c>
+      <c r="V8" t="s">
+        <v>54</v>
+      </c>
+      <c r="W8" t="s">
         <v>117</v>
       </c>
-      <c r="N8" t="s">
-        <v>129</v>
-      </c>
-      <c r="O8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>52</v>
-      </c>
-      <c r="R8" t="s">
-        <v>130</v>
-      </c>
-      <c r="T8" t="s">
-        <v>131</v>
-      </c>
-      <c r="U8" t="s">
-        <v>132</v>
-      </c>
-      <c r="V8" t="s">
-        <v>53</v>
-      </c>
-      <c r="W8" t="s">
-        <v>116</v>
-      </c>
       <c r="X8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Y8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AA8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AC8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AF8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AG8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AH8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AI8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AK8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AL8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L9" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9" t="s">
         <v>118</v>
       </c>
-      <c r="M9" t="s">
-        <v>117</v>
-      </c>
       <c r="N9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Q9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="S9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="T9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W9" t="s">
         <v>69</v>
       </c>
-      <c r="W9" t="s">
-        <v>68</v>
-      </c>
       <c r="X9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Z9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AA9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AC9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AE9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M10" t="s">
         <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="S10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="T10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="U10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="W10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Y10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AA10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AC10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="N11" t="s">
         <v>45</v>
       </c>
       <c r="O11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="T11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Y11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AA11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AB11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AC11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AF11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AG11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AH11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AI11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>169</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>170</v>
+      </c>
+      <c r="AM11" t="s">
         <v>69</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>169</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AA13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AC13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B14" t="s">
-        <v>176</v>
+        <v>181</v>
+      </c>
+      <c r="C14" t="s">
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="G14" t="s">
-        <v>178</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="J14" t="s">
-        <v>153</v>
+        <v>96</v>
+      </c>
+      <c r="K14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M14" t="s">
+        <v>163</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>106</v>
+      </c>
+      <c r="R14" t="s">
+        <v>183</v>
+      </c>
+      <c r="S14" t="s">
+        <v>54</v>
+      </c>
+      <c r="T14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U14" t="s">
+        <v>77</v>
+      </c>
+      <c r="V14" t="s">
+        <v>90</v>
+      </c>
+      <c r="W14" t="s">
+        <v>54</v>
+      </c>
+      <c r="X14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>185</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" t="s">
-        <v>141</v>
-      </c>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L15" t="s">
-        <v>118</v>
-      </c>
-      <c r="M15" t="s">
-        <v>162</v>
-      </c>
-      <c r="N15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" t="s">
-        <v>92</v>
-      </c>
-      <c r="P15" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>105</v>
-      </c>
-      <c r="R15" t="s">
-        <v>183</v>
-      </c>
-      <c r="S15" t="s">
-        <v>53</v>
-      </c>
-      <c r="T15" t="s">
-        <v>95</v>
-      </c>
-      <c r="U15" t="s">
-        <v>76</v>
-      </c>
-      <c r="V15" t="s">
-        <v>89</v>
-      </c>
-      <c r="W15" t="s">
-        <v>53</v>
-      </c>
-      <c r="X15" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>184</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>185</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>193</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>194</v>
+      </c>
+      <c r="G16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" t="s">
+        <v>195</v>
+      </c>
+      <c r="L16" t="s">
+        <v>112</v>
+      </c>
+      <c r="M16" t="s">
+        <v>92</v>
+      </c>
+      <c r="T16" t="s">
+        <v>196</v>
+      </c>
+      <c r="U16" t="s">
+        <v>197</v>
+      </c>
+      <c r="V16" t="s">
+        <v>198</v>
+      </c>
+      <c r="W16" t="s">
+        <v>199</v>
+      </c>
+      <c r="X16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>207</v>
+      </c>
+      <c r="B17" t="s">
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" t="s">
+        <v>198</v>
+      </c>
+      <c r="L17" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" t="s">
+        <v>163</v>
+      </c>
+      <c r="N17" t="s">
+        <v>130</v>
+      </c>
+      <c r="O17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P17" t="s">
         <v>94</v>
       </c>
-      <c r="E17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" t="s">
-        <v>194</v>
-      </c>
-      <c r="G17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" t="s">
-        <v>195</v>
-      </c>
-      <c r="L17" t="s">
-        <v>111</v>
-      </c>
-      <c r="M17" t="s">
-        <v>91</v>
+      <c r="Q17" t="s">
+        <v>106</v>
+      </c>
+      <c r="R17" t="s">
+        <v>107</v>
+      </c>
+      <c r="S17" t="s">
+        <v>147</v>
       </c>
       <c r="T17" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="U17" t="s">
-        <v>197</v>
-      </c>
-      <c r="V17" t="s">
-        <v>198</v>
-      </c>
-      <c r="W17" t="s">
-        <v>199</v>
-      </c>
-      <c r="X17" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>201</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>204</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>205</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>124</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>206</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C18" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>210</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="I18" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J18" t="s">
-        <v>88</v>
-      </c>
-      <c r="K18" t="s">
-        <v>198</v>
-      </c>
-      <c r="L18" t="s">
-        <v>90</v>
-      </c>
-      <c r="M18" t="s">
-        <v>162</v>
+        <v>89</v>
       </c>
       <c r="N18" t="s">
-        <v>129</v>
+        <v>215</v>
       </c>
       <c r="O18" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
       <c r="P18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q18" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="R18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S18" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="T18" t="s">
         <v>211</v>
       </c>
       <c r="U18" t="s">
-        <v>68</v>
+        <v>161</v>
+      </c>
+      <c r="V18" t="s">
+        <v>69</v>
+      </c>
+      <c r="W18" t="s">
+        <v>199</v>
+      </c>
+      <c r="X18" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>169</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="G19" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="H19" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="I19" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="J19" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="N19" t="s">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="O19" t="s">
-        <v>216</v>
+        <v>93</v>
       </c>
       <c r="P19" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="Q19" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="R19" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="S19" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="T19" t="s">
         <v>211</v>
       </c>
       <c r="U19" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="V19" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="W19" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="X19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y19" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="Z19" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="AA19" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="AB19" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="AC19" t="s">
-        <v>218</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>219</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>220</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>221</v>
-      </c>
-      <c r="B20" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C20" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>229</v>
       </c>
       <c r="E20" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="H20" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="J20" t="s">
-        <v>95</v>
-      </c>
-      <c r="N20" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" t="s">
-        <v>92</v>
-      </c>
-      <c r="P20" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>105</v>
-      </c>
-      <c r="R20" t="s">
-        <v>53</v>
-      </c>
-      <c r="S20" t="s">
-        <v>102</v>
-      </c>
-      <c r="T20" t="s">
-        <v>211</v>
-      </c>
-      <c r="U20" t="s">
-        <v>54</v>
-      </c>
-      <c r="V20" t="s">
-        <v>173</v>
-      </c>
-      <c r="W20" t="s">
-        <v>226</v>
-      </c>
-      <c r="X20" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>102</v>
+        <v>59</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>230</v>
+      </c>
+      <c r="B21" t="s">
+        <v>231</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D21" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>178</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>211</v>
       </c>
       <c r="K21" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="L21" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" t="s">
+        <v>63</v>
+      </c>
+      <c r="O21" t="s">
+        <v>64</v>
+      </c>
+      <c r="P21" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>95</v>
+      </c>
+      <c r="R21" t="s">
+        <v>107</v>
+      </c>
+      <c r="S21" t="s">
+        <v>233</v>
+      </c>
+      <c r="T21" t="s">
+        <v>96</v>
+      </c>
+      <c r="U21" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" t="s">
+        <v>54</v>
+      </c>
+      <c r="W21" t="s">
+        <v>234</v>
+      </c>
+      <c r="X21" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C22" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="J22" t="s">
-        <v>211</v>
+        <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="L22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="N22" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="O22" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
       <c r="P22" t="s">
-        <v>64</v>
+        <v>239</v>
       </c>
       <c r="Q22" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="R22" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="S22" t="s">
-        <v>233</v>
+        <v>69</v>
       </c>
       <c r="T22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U22" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="V22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W22" t="s">
-        <v>234</v>
+        <v>54</v>
       </c>
       <c r="X22" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>220</v>
-      </c>
-      <c r="AK22" t="s">
-        <v>205</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>124</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>240</v>
+      </c>
+      <c r="B23" t="s">
+        <v>241</v>
       </c>
       <c r="C23" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" t="s">
+        <v>129</v>
+      </c>
+      <c r="J23" t="s">
+        <v>211</v>
+      </c>
+      <c r="K23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" t="s">
+        <v>64</v>
+      </c>
+      <c r="P23" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q23" t="s">
         <v>53</v>
       </c>
-      <c r="E23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" t="s">
-        <v>237</v>
-      </c>
-      <c r="H23" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" t="s">
-        <v>238</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="R23" t="s">
+        <v>183</v>
+      </c>
+      <c r="S23" t="s">
+        <v>147</v>
+      </c>
+      <c r="T23" t="s">
+        <v>96</v>
+      </c>
+      <c r="U23" t="s">
+        <v>54</v>
+      </c>
+      <c r="V23" t="s">
         <v>90</v>
       </c>
-      <c r="M23" t="s">
+      <c r="W23" t="s">
+        <v>243</v>
+      </c>
+      <c r="X23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA23" t="s">
         <v>91</v>
-      </c>
-      <c r="N23" t="s">
-        <v>142</v>
-      </c>
-      <c r="O23" t="s">
-        <v>216</v>
-      </c>
-      <c r="P23" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>177</v>
-      </c>
-      <c r="R23" t="s">
-        <v>74</v>
-      </c>
-      <c r="S23" t="s">
-        <v>68</v>
-      </c>
-      <c r="T23" t="s">
-        <v>95</v>
-      </c>
-      <c r="U23" t="s">
-        <v>141</v>
-      </c>
-      <c r="V23" t="s">
-        <v>53</v>
-      </c>
-      <c r="W23" t="s">
-        <v>53</v>
-      </c>
-      <c r="X23" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="I24" t="s">
-        <v>128</v>
-      </c>
-      <c r="J24" t="s">
-        <v>211</v>
+        <v>54</v>
       </c>
       <c r="K24" t="s">
-        <v>53</v>
-      </c>
-      <c r="L24" t="s">
-        <v>90</v>
-      </c>
-      <c r="M24" t="s">
-        <v>61</v>
-      </c>
-      <c r="N24" t="s">
-        <v>45</v>
-      </c>
-      <c r="O24" t="s">
-        <v>63</v>
-      </c>
-      <c r="P24" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>52</v>
-      </c>
-      <c r="R24" t="s">
-        <v>183</v>
-      </c>
-      <c r="S24" t="s">
-        <v>146</v>
-      </c>
-      <c r="T24" t="s">
-        <v>95</v>
-      </c>
-      <c r="U24" t="s">
-        <v>53</v>
-      </c>
-      <c r="V24" t="s">
-        <v>89</v>
-      </c>
-      <c r="W24" t="s">
-        <v>243</v>
-      </c>
-      <c r="X24" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA24" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B25" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C25" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" t="s">
-        <v>141</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>250</v>
+      </c>
+      <c r="B26" t="s">
+        <v>251</v>
       </c>
       <c r="C26" t="s">
-        <v>248</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>249</v>
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J26" t="s">
+        <v>211</v>
+      </c>
+      <c r="K26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L26" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" t="s">
+        <v>163</v>
+      </c>
+      <c r="N26" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>53</v>
+      </c>
+      <c r="R26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" t="s">
-        <v>128</v>
-      </c>
-      <c r="J27" t="s">
-        <v>211</v>
-      </c>
-      <c r="K27" t="s">
-        <v>102</v>
-      </c>
-      <c r="L27" t="s">
-        <v>90</v>
-      </c>
-      <c r="M27" t="s">
-        <v>162</v>
-      </c>
-      <c r="N27" t="s">
-        <v>62</v>
-      </c>
-      <c r="O27" t="s">
-        <v>92</v>
-      </c>
-      <c r="P27" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>52</v>
-      </c>
-      <c r="R27" t="s">
-        <v>74</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C28" t="s">
-        <v>254</v>
+        <v>257</v>
+      </c>
+      <c r="K28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>255</v>
-      </c>
-      <c r="B29" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
-        <v>257</v>
-      </c>
-      <c r="K29" t="s">
-        <v>59</v>
+        <v>259</v>
       </c>
       <c r="L29" t="s">
+        <v>119</v>
+      </c>
+      <c r="M29" t="s">
         <v>118</v>
       </c>
-      <c r="M29" t="s">
-        <v>91</v>
+      <c r="N29" t="s">
+        <v>143</v>
+      </c>
+      <c r="P29" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>261</v>
+      </c>
+      <c r="D30" t="s">
+        <v>262</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" t="s">
+        <v>129</v>
+      </c>
+      <c r="J30" t="s">
+        <v>211</v>
+      </c>
+      <c r="K30" t="s">
+        <v>60</v>
       </c>
       <c r="L30" t="s">
+        <v>91</v>
+      </c>
+      <c r="M30" t="s">
         <v>118</v>
       </c>
-      <c r="M30" t="s">
-        <v>117</v>
-      </c>
       <c r="N30" t="s">
-        <v>142</v>
+        <v>45</v>
+      </c>
+      <c r="O30" t="s">
+        <v>64</v>
       </c>
       <c r="P30" t="s">
-        <v>239</v>
+        <v>94</v>
       </c>
       <c r="Q30" t="s">
-        <v>52</v>
+        <v>262</v>
+      </c>
+      <c r="R30" t="s">
+        <v>54</v>
+      </c>
+      <c r="S30" t="s">
+        <v>54</v>
+      </c>
+      <c r="T30" t="s">
+        <v>54</v>
+      </c>
+      <c r="U30" t="s">
+        <v>54</v>
+      </c>
+      <c r="V30" t="s">
+        <v>54</v>
+      </c>
+      <c r="W30" t="s">
+        <v>54</v>
+      </c>
+      <c r="X30" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>263</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>266</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>170</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>260</v>
+        <v>267</v>
+      </c>
+      <c r="B31" t="s">
+        <v>268</v>
       </c>
       <c r="C31" t="s">
-        <v>261</v>
-      </c>
-      <c r="D31" t="s">
-        <v>262</v>
-      </c>
-      <c r="E31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" t="s">
-        <v>86</v>
-      </c>
-      <c r="H31" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" t="s">
-        <v>128</v>
-      </c>
-      <c r="J31" t="s">
-        <v>211</v>
-      </c>
-      <c r="K31" t="s">
+        <v>269</v>
+      </c>
+      <c r="P31" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>95</v>
+      </c>
+      <c r="R31" t="s">
+        <v>107</v>
+      </c>
+      <c r="S31" t="s">
+        <v>68</v>
+      </c>
+      <c r="T31" t="s">
         <v>59</v>
       </c>
-      <c r="L31" t="s">
-        <v>90</v>
-      </c>
-      <c r="M31" t="s">
-        <v>117</v>
-      </c>
-      <c r="N31" t="s">
-        <v>45</v>
-      </c>
-      <c r="O31" t="s">
-        <v>63</v>
-      </c>
-      <c r="P31" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>262</v>
-      </c>
-      <c r="R31" t="s">
-        <v>53</v>
-      </c>
-      <c r="S31" t="s">
-        <v>53</v>
-      </c>
-      <c r="T31" t="s">
-        <v>53</v>
-      </c>
       <c r="U31" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="V31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W31" t="s">
-        <v>53</v>
+        <v>226</v>
       </c>
       <c r="X31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y31" t="s">
-        <v>263</v>
+        <v>46</v>
       </c>
       <c r="Z31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AA31" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>265</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF31" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>266</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI31" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL31" t="s">
-        <v>169</v>
-      </c>
-      <c r="AM31" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
-      </c>
-      <c r="P32" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>94</v>
-      </c>
-      <c r="R32" t="s">
-        <v>106</v>
-      </c>
-      <c r="S32" t="s">
-        <v>67</v>
-      </c>
-      <c r="T32" t="s">
-        <v>58</v>
-      </c>
-      <c r="U32" t="s">
-        <v>114</v>
-      </c>
-      <c r="V32" t="s">
-        <v>53</v>
+        <v>271</v>
+      </c>
+      <c r="D32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" t="s">
+        <v>179</v>
+      </c>
+      <c r="I32" t="s">
+        <v>180</v>
+      </c>
+      <c r="J32" t="s">
+        <v>154</v>
       </c>
       <c r="W32" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="X32" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="Y32" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z32" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="AA32" t="s">
-        <v>111</v>
+        <v>264</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sections for upcoming and old matches and updated the users list
</commit_message>
<xml_diff>
--- a/eventData/users.xlsx
+++ b/eventData/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AU33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -627,6 +627,46 @@
       <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Czech Republic vs Turkey</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Switzerland vs Italy</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Germany vs Denmark</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>England vs Slovakia</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Spain vs Georgia</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>France vs Belgium</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Portugal vs Slovenia</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Romania vs Netherlands</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Austria vs Turkey</t>
         </is>
       </c>
     </row>
@@ -706,6 +746,14 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -759,6 +807,14 @@
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -808,6 +864,14 @@
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1001,6 +1065,14 @@
           <t>['Turkey', 0, 3]</t>
         </is>
       </c>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1190,6 +1262,14 @@
           <t>['Draw', 0, 0]</t>
         </is>
       </c>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1383,6 +1463,14 @@
           <t>['Czech Republic', 2, 0]</t>
         </is>
       </c>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1568,6 +1656,14 @@
           <t>['Draw', 0, 0]</t>
         </is>
       </c>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1761,6 +1857,46 @@
           <t>['Turkey', 1, 2]</t>
         </is>
       </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>['Italy', 1, 2]</t>
+        </is>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>['Germany', 3, 1]</t>
+        </is>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t>['England', 2, 0]</t>
+        </is>
+      </c>
+      <c r="AQ9" t="inlineStr">
+        <is>
+          <t>['Spain', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AR9" t="inlineStr">
+        <is>
+          <t>['France', 2, 0]</t>
+        </is>
+      </c>
+      <c r="AS9" t="inlineStr">
+        <is>
+          <t>['Portugal', 1, 0]</t>
+        </is>
+      </c>
+      <c r="AT9" t="inlineStr">
+        <is>
+          <t>['Netherlands', 1, 2]</t>
+        </is>
+      </c>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t>['Austria', 2, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1938,6 +2074,14 @@
           <t>['Turkey', 1, 2]</t>
         </is>
       </c>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2131,6 +2275,14 @@
           <t>['Draw', 2, 2]</t>
         </is>
       </c>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -2176,6 +2328,14 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2253,6 +2413,14 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2446,6 +2614,14 @@
           <t>['Turkey', 0, 2]</t>
         </is>
       </c>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2495,6 +2671,14 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2664,6 +2848,14 @@
           <t>['Turkey', 2, 3]</t>
         </is>
       </c>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2841,6 +3033,14 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
+      <c r="AS17" t="inlineStr"/>
+      <c r="AT17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3026,6 +3226,14 @@
           <t>['Draw', 1, 1]</t>
         </is>
       </c>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr"/>
+      <c r="AS18" t="inlineStr"/>
+      <c r="AT18" t="inlineStr"/>
+      <c r="AU18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3211,6 +3419,14 @@
           <t>['Draw', 0, 0]</t>
         </is>
       </c>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
+      <c r="AS19" t="inlineStr"/>
+      <c r="AT19" t="inlineStr"/>
+      <c r="AU19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3292,6 +3508,14 @@
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr"/>
+      <c r="AS20" t="inlineStr"/>
+      <c r="AT20" t="inlineStr"/>
+      <c r="AU20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3489,6 +3713,14 @@
           <t>['Czech Republic', 2, 0]</t>
         </is>
       </c>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
+      <c r="AR21" t="inlineStr"/>
+      <c r="AS21" t="inlineStr"/>
+      <c r="AT21" t="inlineStr"/>
+      <c r="AU21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3638,6 +3870,14 @@
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
+      <c r="AR22" t="inlineStr"/>
+      <c r="AS22" t="inlineStr"/>
+      <c r="AT22" t="inlineStr"/>
+      <c r="AU22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3835,6 +4075,14 @@
           <t>['Czech Republic', 1, 0]</t>
         </is>
       </c>
+      <c r="AN23" t="inlineStr"/>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
+      <c r="AR23" t="inlineStr"/>
+      <c r="AS23" t="inlineStr"/>
+      <c r="AT23" t="inlineStr"/>
+      <c r="AU23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3916,6 +4164,14 @@
       <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
+      <c r="AR24" t="inlineStr"/>
+      <c r="AS24" t="inlineStr"/>
+      <c r="AT24" t="inlineStr"/>
+      <c r="AU24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3969,6 +4225,14 @@
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr"/>
       <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
+      <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
+      <c r="AR25" t="inlineStr"/>
+      <c r="AS25" t="inlineStr"/>
+      <c r="AT25" t="inlineStr"/>
+      <c r="AU25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4082,6 +4346,14 @@
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr"/>
       <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
+      <c r="AR26" t="inlineStr"/>
+      <c r="AS26" t="inlineStr"/>
+      <c r="AT26" t="inlineStr"/>
+      <c r="AU26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4135,6 +4407,14 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
+      <c r="AR27" t="inlineStr"/>
+      <c r="AS27" t="inlineStr"/>
+      <c r="AT27" t="inlineStr"/>
+      <c r="AU27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4200,6 +4480,14 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr"/>
       <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" t="inlineStr"/>
+      <c r="AS28" t="inlineStr"/>
+      <c r="AT28" t="inlineStr"/>
+      <c r="AU28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4269,6 +4557,14 @@
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" t="inlineStr"/>
       <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
+      <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="inlineStr"/>
+      <c r="AQ29" t="inlineStr"/>
+      <c r="AR29" t="inlineStr"/>
+      <c r="AS29" t="inlineStr"/>
+      <c r="AT29" t="inlineStr"/>
+      <c r="AU29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4460,6 +4756,46 @@
       <c r="AM30" t="inlineStr">
         <is>
           <t>['Draw', 1, 1]</t>
+        </is>
+      </c>
+      <c r="AN30" t="inlineStr">
+        <is>
+          <t>['Draw', 1, 1]</t>
+        </is>
+      </c>
+      <c r="AO30" t="inlineStr">
+        <is>
+          <t>['Germany', 2, 0]</t>
+        </is>
+      </c>
+      <c r="AP30" t="inlineStr">
+        <is>
+          <t>['England', 1, 0]</t>
+        </is>
+      </c>
+      <c r="AQ30" t="inlineStr">
+        <is>
+          <t>['Spain', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AR30" t="inlineStr">
+        <is>
+          <t>['France', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AS30" t="inlineStr">
+        <is>
+          <t>['Portugal', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AT30" t="inlineStr">
+        <is>
+          <t>['Draw', 1, 1]</t>
+        </is>
+      </c>
+      <c r="AU30" t="inlineStr">
+        <is>
+          <t>['Austria', 2, 1]</t>
         </is>
       </c>
     </row>
@@ -4611,6 +4947,22 @@
           <t>['Czech Republic', 2, 1]</t>
         </is>
       </c>
+      <c r="AN31" t="inlineStr">
+        <is>
+          <t>['Switzerland', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AO31" t="inlineStr">
+        <is>
+          <t>['Germany', 2, 1]</t>
+        </is>
+      </c>
+      <c r="AP31" t="inlineStr"/>
+      <c r="AQ31" t="inlineStr"/>
+      <c r="AR31" t="inlineStr"/>
+      <c r="AS31" t="inlineStr"/>
+      <c r="AT31" t="inlineStr"/>
+      <c r="AU31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4744,6 +5096,99 @@
           <t>['Turkey', 0, 3]</t>
         </is>
       </c>
+      <c r="AN32" t="inlineStr">
+        <is>
+          <t>['Switzerland', 1, 0]</t>
+        </is>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>['Germany', 3, 0]</t>
+        </is>
+      </c>
+      <c r="AP32" t="inlineStr">
+        <is>
+          <t>['England', 2, 0]</t>
+        </is>
+      </c>
+      <c r="AQ32" t="inlineStr">
+        <is>
+          <t>['Spain', 4, 0]</t>
+        </is>
+      </c>
+      <c r="AR32" t="inlineStr">
+        <is>
+          <t>['France', 2, 0]</t>
+        </is>
+      </c>
+      <c r="AS32" t="inlineStr">
+        <is>
+          <t>['Portugal', 1, 0]</t>
+        </is>
+      </c>
+      <c r="AT32" t="inlineStr">
+        <is>
+          <t>['Romania', 1, 0]</t>
+        </is>
+      </c>
+      <c r="AU32" t="inlineStr">
+        <is>
+          <t>['Austria', 2, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
+      <c r="AP33" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
+      <c r="AR33" t="inlineStr"/>
+      <c r="AS33" t="inlineStr"/>
+      <c r="AT33" t="inlineStr"/>
+      <c r="AU33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>